<commit_message>
Update do Readme e criacao do arquivo analises.ipynb com as primeiras analises
</commit_message>
<xml_diff>
--- a/Thanael - Data Glow Up 33.xlsx
+++ b/Thanael - Data Glow Up 33.xlsx
@@ -3,11 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Biggest Oil Producers" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Copy of Who Imports Russian Oil" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Copy of % Dependency on Russian" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Copy of Worlds Proven Oil Reser" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Copy of Who Supports Russia" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="biggest_oil_producers" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="import_russian_oil" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="dependency_russian_oil" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="proven_oil_reserves" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="support_russian" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -1096,7 +1096,7 @@
     <xdr:ext cx="5962650" cy="4857750"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1129,7 +1129,7 @@
     <xdr:ext cx="5810250" cy="5838825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1162,7 +1162,7 @@
     <xdr:ext cx="4210050" cy="5591175"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>